<commit_message>
Add whole-number validations to cells
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_7.xlsx
+++ b/templates/NHWA_Module_7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{9EB1D75C-8781-2440-B4F5-CE5B826D40FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B35A81-3608-2B45-8834-6D283EEB6884}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="dropdownlist">Expenditure!$AE$2:INDEX(Expenditure!$AE$2:$AE$251,MAX(Expenditure!$AD$2:$AD$251),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2720,19 +2719,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2750,6 +2736,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2780,15 +2788,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2831,64 +2830,124 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>711200</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>279400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="ComboBox1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2050" name="ComboBox1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s2050"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="ComboBox1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="863600"/>
+          <a:ext cx="4864100" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3275,12 +3334,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BZ252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3309,16 +3368,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -3349,16 +3408,16 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="42" t="s">
         <v>760</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -3534,13 +3593,13 @@
       </c>
     </row>
     <row r="6" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="40" t="s">
         <v>774</v>
       </c>
       <c r="E6" s="19"/>
@@ -3553,8 +3612,8 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
       <c r="Y6" s="4" t="s">
         <v>16</v>
       </c>
@@ -3581,9 +3640,9 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -3625,7 +3684,7 @@
       <c r="B8" s="20">
         <v>1</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="34" t="s">
         <v>779</v>
       </c>
       <c r="D8" s="21"/>
@@ -3667,9 +3726,9 @@
       </c>
     </row>
     <row r="9" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -3684,17 +3743,17 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="40" t="s">
         <v>761</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
@@ -3707,8 +3766,8 @@
       <c r="T10" s="17"/>
     </row>
     <row r="11" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="28" t="s">
         <v>775</v>
       </c>
@@ -3730,15 +3789,15 @@
       <c r="T11" s="17"/>
     </row>
     <row r="12" spans="2:31" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="40">
-        <v>1</v>
-      </c>
-      <c r="C12" s="38" t="s">
+      <c r="B12" s="36">
+        <v>1</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>778</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
@@ -3792,19 +3851,19 @@
       </c>
     </row>
     <row r="14" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="39" t="s">
         <v>763</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="39" t="s">
         <v>764</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="39" t="s">
         <v>765</v>
       </c>
       <c r="G14" s="19"/>
@@ -3843,11 +3902,11 @@
       </c>
     </row>
     <row r="15" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -3970,19 +4029,19 @@
       </c>
     </row>
     <row r="18" spans="2:32" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="39" t="s">
         <v>770</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="39" t="s">
         <v>780</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="39" t="s">
         <v>765</v>
       </c>
       <c r="G18" s="19"/>
@@ -4020,11 +4079,11 @@
       </c>
     </row>
     <row r="19" spans="2:32" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="M19" s="17"/>
@@ -4063,7 +4122,7 @@
       <c r="B20" s="20">
         <v>1</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="34" t="s">
         <v>781</v>
       </c>
       <c r="D20" s="21"/>
@@ -4104,12 +4163,12 @@
       </c>
     </row>
     <row r="21" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="N21" s="17"/>
@@ -4121,22 +4180,22 @@
       <c r="T21" s="17"/>
     </row>
     <row r="22" spans="2:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="39" t="s">
         <v>767</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="39" t="s">
         <v>768</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="39" t="s">
         <v>769</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="39" t="s">
         <v>758</v>
       </c>
       <c r="H22" s="19"/>
@@ -4168,12 +4227,12 @@
       </c>
     </row>
     <row r="23" spans="2:32" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="Z23" s="4" t="s">
@@ -10203,12 +10262,12 @@
     <protectedRange sqref="I4 P20:Q20 D16:D17 E17:G17 G14:G16 E16:F16 Q21:R21 F20 D8:G13 D24:G24 G25 G18:Q19 H8:R17 D20:E21 F21:G21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="25">
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="B6:B7"/>
@@ -10218,21 +10277,28 @@
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:G24 D20:F20 D16:F16 D12:F12 D8" xr:uid="{49602918-72D9-3E47-A919-4C37502B56A3}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4" xr:uid="{5D81A9CD-EB1F-3241-8A49-6FED392EF4BF}">
+      <formula1>2000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10265,32 +10331,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:17" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="42" t="s">
         <v>760</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -10350,45 +10416,45 @@
       <c r="N6" s="14"/>
     </row>
     <row r="7" spans="2:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="44" t="s">
         <v>782</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="47" t="s">
         <v>771</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="51" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="53" t="s">
         <v>783</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="2:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="2:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="30" t="s">
         <v>775</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>776</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="37" t="s">
         <v>777</v>
       </c>
       <c r="G9" s="29" t="s">
@@ -10415,8 +10481,8 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10506,26 +10572,26 @@
     </row>
     <row r="17" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="40" t="s">
         <v>757</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="40" t="s">
         <v>773</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="40" t="s">
         <v>787</v>
       </c>
-      <c r="F18" s="32"/>
+      <c r="F18" s="40"/>
     </row>
     <row r="19" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="2:15" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="20">
@@ -10535,8 +10601,8 @@
         <v>772</v>
       </c>
       <c r="D20" s="24"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
       <c r="N20" s="14">
         <v>1</v>
       </c>
@@ -10550,18 +10616,26 @@
     <protectedRange sqref="D20" name="Range1_1"/>
   </protectedRanges>
   <mergeCells count="11">
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:F8"/>
     <mergeCell ref="G7:I8"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:I16" xr:uid="{283C7464-3E7C-F949-A54A-11C987824371}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4" xr:uid="{475FCC0D-5B3A-D24F-BDC3-1B4EDB7141DC}">
+      <formula1>2000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>